<commit_message>
Switch Pit and Tank tab names
</commit_message>
<xml_diff>
--- a/modesto/Data/Investment/Storage.xlsx
+++ b/modesto/Data/Investment/Storage.xlsx
@@ -5,23 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0094934\Research\modesto\modesto\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0094934\Research\modesto\modesto\Data\Investment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
   </bookViews>
   <sheets>
-    <sheet name="Pit" sheetId="1" r:id="rId1"/>
-    <sheet name="Tank" sheetId="2" r:id="rId2"/>
+    <sheet name="Tank" sheetId="1" r:id="rId1"/>
+    <sheet name="Pit" sheetId="2" r:id="rId2"/>
     <sheet name="Borehole" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Borehole!$A$3:$A$6</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Borehole!$B$3:$B$6</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Borehole!$A$2:$A$5</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Borehole!$B$2:$B$5</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -158,7 +152,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Pit!$B$1</c:f>
+              <c:f>Tank!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -193,7 +187,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Pit!$A$2:$A$9</c:f>
+              <c:f>Tank!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -226,7 +220,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Pit!$B$2:$B$9</c:f>
+              <c:f>Tank!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -500,7 +494,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tank!$B$1</c:f>
+              <c:f>Pit!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -535,7 +529,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tank!$A$2:$A$9</c:f>
+              <c:f>Pit!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -568,7 +562,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tank!$B$2:$B$9</c:f>
+              <c:f>Pit!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -3149,12 +3143,12 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3162,7 +3156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3170,7 +3164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>300</v>
       </c>
@@ -3178,7 +3172,7 @@
         <v>139500</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>480</v>
       </c>
@@ -3186,7 +3180,7 @@
         <v>230400</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>600</v>
       </c>
@@ -3194,7 +3188,7 @@
         <v>273000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2750</v>
       </c>
@@ -3202,7 +3196,7 @@
         <v>660000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>4500</v>
       </c>
@@ -3210,7 +3204,7 @@
         <v>945000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>5750</v>
       </c>
@@ -3218,7 +3212,7 @@
         <v>948750</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>11700</v>
       </c>
@@ -3240,9 +3234,9 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3250,7 +3244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -3258,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>725</v>
       </c>
@@ -3266,7 +3260,7 @@
         <v>177625</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3000</v>
       </c>
@@ -3274,7 +3268,7 @@
         <v>435000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>5400</v>
       </c>
@@ -3282,7 +3276,7 @@
         <v>631800</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>10000</v>
       </c>
@@ -3290,7 +3284,7 @@
         <v>770000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>50000</v>
       </c>
@@ -3298,7 +3292,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>125000</v>
       </c>
@@ -3306,7 +3300,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>200000</v>
       </c>
@@ -3328,9 +3322,9 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3338,7 +3332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -3346,7 +3340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>4500</v>
       </c>
@@ -3354,7 +3348,7 @@
         <v>238500</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>5000</v>
       </c>
@@ -3362,7 +3356,7 @@
         <v>460000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>10100</v>
       </c>
@@ -3370,7 +3364,7 @@
         <v>505000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>16000</v>
       </c>

</xml_diff>